<commit_message>
Ensure exceldata.xlsx with 'data' sheet is committed
</commit_message>
<xml_diff>
--- a/target/test-classes/exceldata.xlsx
+++ b/target/test-classes/exceldata.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Niharika Chauhan\eclipse-workspace\TestNg_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{182BB129-9721-4ABD-856F-3CA8D307375A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F7009181-B467-418E-AB34-CEE5D7AA23A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{085CDAFF-8E72-4B5C-80D7-8F145528770F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -27,16 +36,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>UserName</t>
+    <t>secret_sauce</t>
+  </si>
+  <si>
+    <t>standard_user</t>
   </si>
   <si>
     <t>Password</t>
   </si>
   <si>
-    <t>standard_user</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
+    <t>UserName</t>
   </si>
 </sst>
 </file>
@@ -108,7 +117,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -120,7 +129,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -167,6 +176,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -202,6 +228,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -353,29 +396,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2E7CD4D-EA3D-49C4-80E6-F64E234E2BC8}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>